<commit_message>
Added updated data to namhak24.dat
</commit_message>
<xml_diff>
--- a/mods/data/HakeAbundanceAtAgeData90_24.xlsx
+++ b/mods/data/HakeAbundanceAtAgeData90_24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/_mymods/Namibian hake/Model/NamibianHake/mods/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9D3401-91F1-484D-9F97-7AF734E05DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B769DE90-65A2-3045-B2A3-1E5199B5C9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{8020282F-626F-4FD1-8F48-B44A974EFDAF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{8020282F-626F-4FD1-8F48-B44A974EFDAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -2706,10 +2706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3038785B-5C10-436B-ACF6-31AE3CDCBF28}">
-  <dimension ref="A1:AS207"/>
+  <dimension ref="A1:BG207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3:AS73"/>
+    <sheetView tabSelected="1" topLeftCell="AC18" workbookViewId="0">
+      <selection activeCell="BG39" sqref="AW39:BG73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6651,7 +6651,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>30</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>31</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>32</v>
       </c>
@@ -7041,7 +7041,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>33</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>34</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:59" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>35</v>
       </c>
@@ -7423,12 +7423,15 @@
         <v>423</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:59" x14ac:dyDescent="0.2">
       <c r="E39" t="s">
         <v>36</v>
       </c>
       <c r="P39" t="s">
         <v>37</v>
+      </c>
+      <c r="AG39">
+        <v>50</v>
       </c>
       <c r="AH39">
         <v>1990</v>
@@ -7477,8 +7480,42 @@
         <f t="shared" ref="AS39:AS73" si="23">AE4</f>
         <v>New</v>
       </c>
-    </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW39">
+        <v>50</v>
+      </c>
+      <c r="AX39">
+        <v>1990</v>
+      </c>
+      <c r="AY39">
+        <v>3.727062453714293E-2</v>
+      </c>
+      <c r="AZ39">
+        <v>0.32392485525338149</v>
+      </c>
+      <c r="BA39">
+        <v>0.39305803308377113</v>
+      </c>
+      <c r="BB39">
+        <v>0.18088337840376312</v>
+      </c>
+      <c r="BC39">
+        <v>4.9160698609136799E-2</v>
+      </c>
+      <c r="BD39">
+        <v>9.8590890584729137E-3</v>
+      </c>
+      <c r="BE39">
+        <v>3.5786989799880737E-3</v>
+      </c>
+      <c r="BF39">
+        <v>1.2727516012737254E-3</v>
+      </c>
+      <c r="BG39">
+        <f>SUM(AQ39:AR39)</f>
+        <v>9.9187047306966932E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -7532,6 +7569,9 @@
       </c>
       <c r="R40" t="s">
         <v>41</v>
+      </c>
+      <c r="AG40">
+        <v>50</v>
       </c>
       <c r="AH40">
         <v>1991</v>
@@ -7580,8 +7620,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW40">
+        <v>50</v>
+      </c>
+      <c r="AX40">
+        <v>1991</v>
+      </c>
+      <c r="AY40">
+        <v>5.3744784267503948E-3</v>
+      </c>
+      <c r="AZ40">
+        <v>0.22185582070304419</v>
+      </c>
+      <c r="BA40">
+        <v>0.28381858508964514</v>
+      </c>
+      <c r="BB40">
+        <v>0.28468393063863473</v>
+      </c>
+      <c r="BC40">
+        <v>0.11580718235070149</v>
+      </c>
+      <c r="BD40">
+        <v>5.5150809600606504E-2</v>
+      </c>
+      <c r="BE40">
+        <v>1.7021133952072279E-2</v>
+      </c>
+      <c r="BF40">
+        <v>9.6756392675755639E-3</v>
+      </c>
+      <c r="BG40">
+        <f t="shared" ref="BG40:BG73" si="24">SUM(AQ40:AR40)</f>
+        <v>6.6124199709695092E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -7635,6 +7709,9 @@
       </c>
       <c r="R41" t="s">
         <v>45</v>
+      </c>
+      <c r="AG41">
+        <v>50</v>
       </c>
       <c r="AH41">
         <v>1992</v>
@@ -7683,8 +7760,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW41">
+        <v>50</v>
+      </c>
+      <c r="AX41">
+        <v>1992</v>
+      </c>
+      <c r="AY41">
+        <v>0.11041867842184458</v>
+      </c>
+      <c r="AZ41">
+        <v>0.48872920505504125</v>
+      </c>
+      <c r="BA41">
+        <v>0.1866117179055026</v>
+      </c>
+      <c r="BB41">
+        <v>7.3995935878509236E-2</v>
+      </c>
+      <c r="BC41">
+        <v>5.7924112224897385E-2</v>
+      </c>
+      <c r="BD41">
+        <v>4.9166163191221475E-2</v>
+      </c>
+      <c r="BE41">
+        <v>1.0751121740273106E-2</v>
+      </c>
+      <c r="BF41">
+        <v>1.1866944216819287E-2</v>
+      </c>
+      <c r="BG41">
+        <f t="shared" si="24"/>
+        <v>1.0536121365891011E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -7738,6 +7849,9 @@
       </c>
       <c r="R42" t="s">
         <v>49</v>
+      </c>
+      <c r="AG42">
+        <v>50</v>
       </c>
       <c r="AH42">
         <v>1993</v>
@@ -7786,8 +7900,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW42">
+        <v>50</v>
+      </c>
+      <c r="AX42">
+        <v>1993</v>
+      </c>
+      <c r="AY42">
+        <v>0</v>
+      </c>
+      <c r="AZ42">
+        <v>4.9397259551487119E-2</v>
+      </c>
+      <c r="BA42">
+        <v>0.56414323400854405</v>
+      </c>
+      <c r="BB42">
+        <v>0.26805339696375935</v>
+      </c>
+      <c r="BC42">
+        <v>5.768260565933922E-2</v>
+      </c>
+      <c r="BD42">
+        <v>3.6293367023270372E-2</v>
+      </c>
+      <c r="BE42">
+        <v>1.8174606643458057E-2</v>
+      </c>
+      <c r="BF42">
+        <v>5.6699163148413011E-3</v>
+      </c>
+      <c r="BG42">
+        <f t="shared" si="24"/>
+        <v>5.8561383530039961E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -7841,6 +7989,9 @@
       </c>
       <c r="R43" t="s">
         <v>53</v>
+      </c>
+      <c r="AG43">
+        <v>50</v>
       </c>
       <c r="AH43">
         <v>1994</v>
@@ -7889,8 +8040,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW43">
+        <v>50</v>
+      </c>
+      <c r="AX43">
+        <v>1994</v>
+      </c>
+      <c r="AY43">
+        <v>1.5865995266475131E-2</v>
+      </c>
+      <c r="AZ43">
+        <v>0.34897650086120918</v>
+      </c>
+      <c r="BA43">
+        <v>0.35956049334085954</v>
+      </c>
+      <c r="BB43">
+        <v>0.13945784911121845</v>
+      </c>
+      <c r="BC43">
+        <v>5.9233377161107201E-2</v>
+      </c>
+      <c r="BD43">
+        <v>3.7822426866589993E-2</v>
+      </c>
+      <c r="BE43">
+        <v>1.9541383860778545E-2</v>
+      </c>
+      <c r="BF43">
+        <v>9.4511567816735094E-3</v>
+      </c>
+      <c r="BG43">
+        <f t="shared" si="24"/>
+        <v>1.0090816750088237E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -7944,6 +8129,9 @@
       </c>
       <c r="R44" t="s">
         <v>57</v>
+      </c>
+      <c r="AG44">
+        <v>50</v>
       </c>
       <c r="AH44">
         <v>1995</v>
@@ -7992,8 +8180,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW44">
+        <v>50</v>
+      </c>
+      <c r="AX44">
+        <v>1995</v>
+      </c>
+      <c r="AY44">
+        <v>4.2460769895567713E-2</v>
+      </c>
+      <c r="AZ44">
+        <v>0.40217028491139528</v>
+      </c>
+      <c r="BA44">
+        <v>0.32297179397655407</v>
+      </c>
+      <c r="BB44">
+        <v>0.11955653099484119</v>
+      </c>
+      <c r="BC44">
+        <v>6.0374783012586621E-2</v>
+      </c>
+      <c r="BD44">
+        <v>2.7643515832749273E-2</v>
+      </c>
+      <c r="BE44">
+        <v>1.2479850886260796E-2</v>
+      </c>
+      <c r="BF44">
+        <v>5.7998827462666276E-3</v>
+      </c>
+      <c r="BG44">
+        <f t="shared" si="24"/>
+        <v>6.5425877437786349E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -8047,6 +8269,9 @@
       </c>
       <c r="R45" t="s">
         <v>61</v>
+      </c>
+      <c r="AG45">
+        <v>50</v>
       </c>
       <c r="AH45">
         <v>1996</v>
@@ -8095,8 +8320,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW45">
+        <v>50</v>
+      </c>
+      <c r="AX45">
+        <v>1996</v>
+      </c>
+      <c r="AY45">
+        <v>0.10489157621612395</v>
+      </c>
+      <c r="AZ45">
+        <v>0.24294968583352458</v>
+      </c>
+      <c r="BA45">
+        <v>0.33271928866526262</v>
+      </c>
+      <c r="BB45">
+        <v>0.18331903487229412</v>
+      </c>
+      <c r="BC45">
+        <v>7.1719865930508858E-2</v>
+      </c>
+      <c r="BD45">
+        <v>3.7299702977544626E-2</v>
+      </c>
+      <c r="BE45">
+        <v>1.6223234730562103E-2</v>
+      </c>
+      <c r="BF45">
+        <v>6.6514954825074458E-3</v>
+      </c>
+      <c r="BG45">
+        <f t="shared" si="24"/>
+        <v>4.2261152916717674E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -8150,6 +8409,9 @@
       </c>
       <c r="R46" t="s">
         <v>65</v>
+      </c>
+      <c r="AG46">
+        <v>50</v>
       </c>
       <c r="AH46">
         <v>1997</v>
@@ -8198,8 +8460,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW46">
+        <v>50</v>
+      </c>
+      <c r="AX46">
+        <v>1997</v>
+      </c>
+      <c r="AY46">
+        <v>6.9493969601829774E-3</v>
+      </c>
+      <c r="AZ46">
+        <v>0.15122983009304983</v>
+      </c>
+      <c r="BA46">
+        <v>0.32603662436609493</v>
+      </c>
+      <c r="BB46">
+        <v>0.29640490725505703</v>
+      </c>
+      <c r="BC46">
+        <v>0.12639670088429508</v>
+      </c>
+      <c r="BD46">
+        <v>5.6330539898568462E-2</v>
+      </c>
+      <c r="BE46">
+        <v>2.2264765171300552E-2</v>
+      </c>
+      <c r="BF46">
+        <v>8.4331156499314157E-3</v>
+      </c>
+      <c r="BG46">
+        <f t="shared" si="24"/>
+        <v>5.9541197215199262E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -8253,6 +8549,9 @@
       </c>
       <c r="R47" t="s">
         <v>69</v>
+      </c>
+      <c r="AG47">
+        <v>50</v>
       </c>
       <c r="AH47">
         <v>1998</v>
@@ -8301,8 +8600,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW47">
+        <v>50</v>
+      </c>
+      <c r="AX47">
+        <v>1998</v>
+      </c>
+      <c r="AY47">
+        <v>4.5163106755578296E-2</v>
+      </c>
+      <c r="AZ47">
+        <v>0.36836587340102916</v>
+      </c>
+      <c r="BA47">
+        <v>0.34760909372647758</v>
+      </c>
+      <c r="BB47">
+        <v>0.12568035058126184</v>
+      </c>
+      <c r="BC47">
+        <v>6.7613311329257242E-2</v>
+      </c>
+      <c r="BD47">
+        <v>2.9404177228012172E-2</v>
+      </c>
+      <c r="BE47">
+        <v>1.0262480543545054E-2</v>
+      </c>
+      <c r="BF47">
+        <v>3.5302312125834279E-3</v>
+      </c>
+      <c r="BG47">
+        <f t="shared" si="24"/>
+        <v>2.3713752222551589E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -8356,6 +8689,9 @@
       </c>
       <c r="R48" t="s">
         <v>73</v>
+      </c>
+      <c r="AG48">
+        <v>50</v>
       </c>
       <c r="AH48">
         <v>1999</v>
@@ -8404,8 +8740,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW48">
+        <v>50</v>
+      </c>
+      <c r="AX48">
+        <v>1999</v>
+      </c>
+      <c r="AY48">
+        <v>0.25275200567553718</v>
+      </c>
+      <c r="AZ48">
+        <v>0.26664861366227705</v>
+      </c>
+      <c r="BA48">
+        <v>0.29895066831583178</v>
+      </c>
+      <c r="BB48">
+        <v>0.11453433692841271</v>
+      </c>
+      <c r="BC48">
+        <v>4.1503960295232137E-2</v>
+      </c>
+      <c r="BD48">
+        <v>1.6601764666269395E-2</v>
+      </c>
+      <c r="BE48">
+        <v>5.0045475325028376E-3</v>
+      </c>
+      <c r="BF48">
+        <v>2.6638641007498353E-3</v>
+      </c>
+      <c r="BG48">
+        <f t="shared" si="24"/>
+        <v>1.3402388231869677E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -8459,6 +8829,9 @@
       </c>
       <c r="R49" t="s">
         <v>77</v>
+      </c>
+      <c r="AG49">
+        <v>50</v>
       </c>
       <c r="AH49">
         <v>2000</v>
@@ -8507,8 +8880,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW49">
+        <v>50</v>
+      </c>
+      <c r="AX49">
+        <v>2000</v>
+      </c>
+      <c r="AY49">
+        <v>2.189082806615401E-2</v>
+      </c>
+      <c r="AZ49">
+        <v>0.21327432038452329</v>
+      </c>
+      <c r="BA49">
+        <v>0.55540554552175481</v>
+      </c>
+      <c r="BB49">
+        <v>0.15860026267412342</v>
+      </c>
+      <c r="BC49">
+        <v>2.0719267235781109E-2</v>
+      </c>
+      <c r="BD49">
+        <v>2.3207170379487264E-2</v>
+      </c>
+      <c r="BE49">
+        <v>4.2584526647000669E-3</v>
+      </c>
+      <c r="BF49">
+        <v>2.4480287801554017E-3</v>
+      </c>
+      <c r="BG49">
+        <f t="shared" si="24"/>
+        <v>1.9612429332049907E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -8562,6 +8969,9 @@
       </c>
       <c r="R50" t="s">
         <v>81</v>
+      </c>
+      <c r="AG50">
+        <v>50</v>
       </c>
       <c r="AH50">
         <v>2001</v>
@@ -8610,8 +9020,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW50">
+        <v>50</v>
+      </c>
+      <c r="AX50">
+        <v>2001</v>
+      </c>
+      <c r="AY50">
+        <v>9.2599622516028962E-2</v>
+      </c>
+      <c r="AZ50">
+        <v>0.16875663881168401</v>
+      </c>
+      <c r="BA50">
+        <v>0.43387397365466451</v>
+      </c>
+      <c r="BB50">
+        <v>0.20487869234115974</v>
+      </c>
+      <c r="BC50">
+        <v>5.6050848584183195E-2</v>
+      </c>
+      <c r="BD50">
+        <v>3.1071792211515608E-2</v>
+      </c>
+      <c r="BE50">
+        <v>7.8324162076766502E-3</v>
+      </c>
+      <c r="BF50">
+        <v>3.5281797500391582E-3</v>
+      </c>
+      <c r="BG50">
+        <f t="shared" si="24"/>
+        <v>1.4078359230480415E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -8665,6 +9109,9 @@
       </c>
       <c r="R51" t="s">
         <v>85</v>
+      </c>
+      <c r="AG51">
+        <v>50</v>
       </c>
       <c r="AH51">
         <v>2002</v>
@@ -8713,8 +9160,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW51">
+        <v>50</v>
+      </c>
+      <c r="AX51">
+        <v>2002</v>
+      </c>
+      <c r="AY51">
+        <v>0.32972570630909498</v>
+      </c>
+      <c r="AZ51">
+        <v>0.52932109011889061</v>
+      </c>
+      <c r="BA51">
+        <v>0.11050232147142962</v>
+      </c>
+      <c r="BB51">
+        <v>1.1423521107427659E-2</v>
+      </c>
+      <c r="BC51">
+        <v>1.1810935554424815E-2</v>
+      </c>
+      <c r="BD51">
+        <v>3.8029590631755415E-3</v>
+      </c>
+      <c r="BE51">
+        <v>1.960488202964317E-3</v>
+      </c>
+      <c r="BF51">
+        <v>8.9555397153476973E-4</v>
+      </c>
+      <c r="BG51">
+        <f t="shared" si="24"/>
+        <v>5.5742420105750598E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -8768,6 +9249,9 @@
       </c>
       <c r="R52" t="s">
         <v>89</v>
+      </c>
+      <c r="AG52">
+        <v>50</v>
       </c>
       <c r="AH52">
         <v>2003</v>
@@ -8816,8 +9300,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW52">
+        <v>50</v>
+      </c>
+      <c r="AX52">
+        <v>2003</v>
+      </c>
+      <c r="AY52">
+        <v>4.0329706530049053E-2</v>
+      </c>
+      <c r="AZ52">
+        <v>0.36470134630796153</v>
+      </c>
+      <c r="BA52">
+        <v>0.36575352368261377</v>
+      </c>
+      <c r="BB52">
+        <v>0.16634206397025636</v>
+      </c>
+      <c r="BC52">
+        <v>4.4460898144272412E-2</v>
+      </c>
+      <c r="BD52">
+        <v>1.2323315511225407E-2</v>
+      </c>
+      <c r="BE52">
+        <v>3.2482804052583309E-3</v>
+      </c>
+      <c r="BF52">
+        <v>8.221644075772608E-4</v>
+      </c>
+      <c r="BG52">
+        <f t="shared" si="24"/>
+        <v>2.0187010407856434E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -8871,6 +9389,9 @@
       </c>
       <c r="R53" t="s">
         <v>93</v>
+      </c>
+      <c r="AG53">
+        <v>50</v>
       </c>
       <c r="AH53">
         <v>2004</v>
@@ -8919,8 +9440,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW53">
+        <v>50</v>
+      </c>
+      <c r="AX53">
+        <v>2004</v>
+      </c>
+      <c r="AY53">
+        <v>5.0324762181524658E-2</v>
+      </c>
+      <c r="AZ53">
+        <v>0.6561509191377719</v>
+      </c>
+      <c r="BA53">
+        <v>0.22850972786981844</v>
+      </c>
+      <c r="BB53">
+        <v>4.3061340089657715E-2</v>
+      </c>
+      <c r="BC53">
+        <v>1.539678967140252E-2</v>
+      </c>
+      <c r="BD53">
+        <v>4.5493395031605153E-3</v>
+      </c>
+      <c r="BE53">
+        <v>1.4621897432557985E-3</v>
+      </c>
+      <c r="BF53">
+        <v>3.7594346970806547E-4</v>
+      </c>
+      <c r="BG53">
+        <f t="shared" si="24"/>
+        <v>1.6898833370072386E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -8974,6 +9529,9 @@
       </c>
       <c r="R54" t="s">
         <v>97</v>
+      </c>
+      <c r="AG54">
+        <v>50</v>
       </c>
       <c r="AH54">
         <v>2005</v>
@@ -9022,8 +9580,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW54">
+        <v>50</v>
+      </c>
+      <c r="AX54">
+        <v>2005</v>
+      </c>
+      <c r="AY54">
+        <v>2.0471068444833228E-4</v>
+      </c>
+      <c r="AZ54">
+        <v>6.714553775305534E-3</v>
+      </c>
+      <c r="BA54">
+        <v>0.33950114158176792</v>
+      </c>
+      <c r="BB54">
+        <v>0.49576638891044167</v>
+      </c>
+      <c r="BC54">
+        <v>0.10129496983468549</v>
+      </c>
+      <c r="BD54">
+        <v>4.1741947700207081E-2</v>
+      </c>
+      <c r="BE54">
+        <v>1.1707173702193926E-2</v>
+      </c>
+      <c r="BF54">
+        <v>1.4396628661730627E-3</v>
+      </c>
+      <c r="BG54">
+        <f t="shared" si="24"/>
+        <v>1.6294509447770621E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -9077,6 +9669,9 @@
       </c>
       <c r="R55" t="s">
         <v>101</v>
+      </c>
+      <c r="AG55">
+        <v>50</v>
       </c>
       <c r="AH55">
         <v>2006</v>
@@ -9125,8 +9720,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW55">
+        <v>50</v>
+      </c>
+      <c r="AX55">
+        <v>2006</v>
+      </c>
+      <c r="AY55">
+        <v>7.5948820053416903E-4</v>
+      </c>
+      <c r="AZ55">
+        <v>0.12648893205836093</v>
+      </c>
+      <c r="BA55">
+        <v>0.57779246642685955</v>
+      </c>
+      <c r="BB55">
+        <v>0.21773300398716333</v>
+      </c>
+      <c r="BC55">
+        <v>6.1682786010898237E-2</v>
+      </c>
+      <c r="BD55">
+        <v>1.1881124734954521E-2</v>
+      </c>
+      <c r="BE55">
+        <v>2.9965926765841786E-3</v>
+      </c>
+      <c r="BF55">
+        <v>5.2460839641883415E-4</v>
+      </c>
+      <c r="BG55">
+        <f t="shared" si="24"/>
+        <v>1.4099750822626307E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -9180,6 +9809,9 @@
       </c>
       <c r="R56" t="s">
         <v>105</v>
+      </c>
+      <c r="AG56">
+        <v>50</v>
       </c>
       <c r="AH56">
         <v>2007</v>
@@ -9228,8 +9860,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW56">
+        <v>50</v>
+      </c>
+      <c r="AX56">
+        <v>2007</v>
+      </c>
+      <c r="AY56">
+        <v>6.9018874450596096E-3</v>
+      </c>
+      <c r="AZ56">
+        <v>0.70134720755693569</v>
+      </c>
+      <c r="BA56">
+        <v>0.20952504487257531</v>
+      </c>
+      <c r="BB56">
+        <v>5.0963052268385912E-2</v>
+      </c>
+      <c r="BC56">
+        <v>2.0132178506124379E-2</v>
+      </c>
+      <c r="BD56">
+        <v>6.2346269898344757E-3</v>
+      </c>
+      <c r="BE56">
+        <v>2.7697376045309669E-3</v>
+      </c>
+      <c r="BF56">
+        <v>1.5813539152077299E-3</v>
+      </c>
+      <c r="BG56">
+        <f t="shared" si="24"/>
+        <v>5.4491084134583676E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -9283,6 +9949,9 @@
       </c>
       <c r="R57" t="s">
         <v>109</v>
+      </c>
+      <c r="AG57">
+        <v>50</v>
       </c>
       <c r="AH57">
         <v>2008</v>
@@ -9331,8 +10000,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW57">
+        <v>50</v>
+      </c>
+      <c r="AX57">
+        <v>2008</v>
+      </c>
+      <c r="AY57">
+        <v>0.24153545811609647</v>
+      </c>
+      <c r="AZ57">
+        <v>0.24259605238594006</v>
+      </c>
+      <c r="BA57">
+        <v>0.2907468779373143</v>
+      </c>
+      <c r="BB57">
+        <v>0.14426121659273736</v>
+      </c>
+      <c r="BC57">
+        <v>4.7581835445021821E-2</v>
+      </c>
+      <c r="BD57">
+        <v>2.2110736816257272E-2</v>
+      </c>
+      <c r="BE57">
+        <v>7.4031929541975572E-3</v>
+      </c>
+      <c r="BF57">
+        <v>2.1161622975014124E-3</v>
+      </c>
+      <c r="BG57">
+        <f t="shared" si="24"/>
+        <v>1.6484674549337741E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>110</v>
       </c>
@@ -9386,6 +10089,9 @@
       </c>
       <c r="R58" t="s">
         <v>113</v>
+      </c>
+      <c r="AG58">
+        <v>50</v>
       </c>
       <c r="AH58">
         <v>2009</v>
@@ -9434,8 +10140,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW58">
+        <v>50</v>
+      </c>
+      <c r="AX58">
+        <v>2009</v>
+      </c>
+      <c r="AY58">
+        <v>6.8889076614307626E-2</v>
+      </c>
+      <c r="AZ58">
+        <v>0.50059751175167699</v>
+      </c>
+      <c r="BA58">
+        <v>0.31555131420587879</v>
+      </c>
+      <c r="BB58">
+        <v>6.3940294204788417E-2</v>
+      </c>
+      <c r="BC58">
+        <v>2.4661372237797758E-2</v>
+      </c>
+      <c r="BD58">
+        <v>1.3267346144626112E-2</v>
+      </c>
+      <c r="BE58">
+        <v>7.8684986810087804E-3</v>
+      </c>
+      <c r="BF58">
+        <v>2.6685576398537796E-3</v>
+      </c>
+      <c r="BG58">
+        <f t="shared" si="24"/>
+        <v>2.5560285200616545E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -9489,6 +10229,9 @@
       </c>
       <c r="R59" t="s">
         <v>117</v>
+      </c>
+      <c r="AG59">
+        <v>50</v>
       </c>
       <c r="AH59">
         <v>2010</v>
@@ -9537,8 +10280,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW59">
+        <v>50</v>
+      </c>
+      <c r="AX59">
+        <v>2010</v>
+      </c>
+      <c r="AY59">
+        <v>0.19627433075364711</v>
+      </c>
+      <c r="AZ59">
+        <v>0.15210955187077876</v>
+      </c>
+      <c r="BA59">
+        <v>0.52425307001553589</v>
+      </c>
+      <c r="BB59">
+        <v>0.10203042941846159</v>
+      </c>
+      <c r="BC59">
+        <v>2.0093139167484137E-2</v>
+      </c>
+      <c r="BD59">
+        <v>4.4319603641045412E-3</v>
+      </c>
+      <c r="BE59">
+        <v>5.6386467653658833E-4</v>
+      </c>
+      <c r="BF59">
+        <v>1.8906022127284524E-4</v>
+      </c>
+      <c r="BG59">
+        <f t="shared" si="24"/>
+        <v>5.4593512178610745E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -9592,6 +10369,9 @@
       </c>
       <c r="R60" t="s">
         <v>121</v>
+      </c>
+      <c r="AG60">
+        <v>50</v>
       </c>
       <c r="AH60">
         <v>2011</v>
@@ -9640,8 +10420,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW60">
+        <v>50</v>
+      </c>
+      <c r="AX60">
+        <v>2011</v>
+      </c>
+      <c r="AY60">
+        <v>0.1979005606341937</v>
+      </c>
+      <c r="AZ60">
+        <v>0.32584404772482101</v>
+      </c>
+      <c r="BA60">
+        <v>0.28672433906667999</v>
+      </c>
+      <c r="BB60">
+        <v>0.10372227344163482</v>
+      </c>
+      <c r="BC60">
+        <v>4.2678623429384374E-2</v>
+      </c>
+      <c r="BD60">
+        <v>2.1314771123615364E-2</v>
+      </c>
+      <c r="BE60">
+        <v>1.3392220309370919E-2</v>
+      </c>
+      <c r="BF60">
+        <v>4.5350120704133615E-3</v>
+      </c>
+      <c r="BG60">
+        <f t="shared" si="24"/>
+        <v>3.8881521998863824E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -9695,6 +10509,9 @@
       </c>
       <c r="R61" t="s">
         <v>125</v>
+      </c>
+      <c r="AG61">
+        <v>50</v>
       </c>
       <c r="AH61">
         <v>2012</v>
@@ -9743,8 +10560,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW61">
+        <v>50</v>
+      </c>
+      <c r="AX61">
+        <v>2012</v>
+      </c>
+      <c r="AY61">
+        <v>0.40263231637456154</v>
+      </c>
+      <c r="AZ61">
+        <v>0.159928670583937</v>
+      </c>
+      <c r="BA61">
+        <v>0.31914829833266667</v>
+      </c>
+      <c r="BB61">
+        <v>5.8129326039919299E-2</v>
+      </c>
+      <c r="BC61">
+        <v>3.3158662030979572E-2</v>
+      </c>
+      <c r="BD61">
+        <v>1.4298260714735169E-2</v>
+      </c>
+      <c r="BE61">
+        <v>6.6633844371397875E-3</v>
+      </c>
+      <c r="BF61">
+        <v>1.914637550104866E-3</v>
+      </c>
+      <c r="BG61">
+        <f t="shared" si="24"/>
+        <v>4.1264439359561152E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>126</v>
       </c>
@@ -9798,6 +10649,9 @@
       </c>
       <c r="R62" t="s">
         <v>129</v>
+      </c>
+      <c r="AG62">
+        <v>50</v>
       </c>
       <c r="AH62">
         <v>2013</v>
@@ -9846,8 +10700,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW62">
+        <v>50</v>
+      </c>
+      <c r="AX62">
+        <v>2013</v>
+      </c>
+      <c r="AY62">
+        <v>5.5388579294062774E-2</v>
+      </c>
+      <c r="AZ62">
+        <v>0.31149245327601305</v>
+      </c>
+      <c r="BA62">
+        <v>0.4621167036500704</v>
+      </c>
+      <c r="BB62">
+        <v>0.13224026276035097</v>
+      </c>
+      <c r="BC62">
+        <v>2.3833852240824096E-2</v>
+      </c>
+      <c r="BD62">
+        <v>9.0341769826409648E-3</v>
+      </c>
+      <c r="BE62">
+        <v>3.0190290787637836E-3</v>
+      </c>
+      <c r="BF62">
+        <v>1.2551348663398267E-3</v>
+      </c>
+      <c r="BG62">
+        <f t="shared" si="24"/>
+        <v>1.61980785093423E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>130</v>
       </c>
@@ -9901,6 +10789,9 @@
       </c>
       <c r="R63" t="s">
         <v>133</v>
+      </c>
+      <c r="AG63">
+        <v>50</v>
       </c>
       <c r="AH63">
         <v>2014</v>
@@ -9949,8 +10840,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW63">
+        <v>50</v>
+      </c>
+      <c r="AX63">
+        <v>2014</v>
+      </c>
+      <c r="AY63">
+        <v>6.6863797425652072E-2</v>
+      </c>
+      <c r="AZ63">
+        <v>0.44908361830264099</v>
+      </c>
+      <c r="BA63">
+        <v>0.32198014298695254</v>
+      </c>
+      <c r="BB63">
+        <v>8.8360316446118525E-2</v>
+      </c>
+      <c r="BC63">
+        <v>3.5057749993723207E-2</v>
+      </c>
+      <c r="BD63">
+        <v>2.1939829753226003E-2</v>
+      </c>
+      <c r="BE63">
+        <v>1.192652505876763E-2</v>
+      </c>
+      <c r="BF63">
+        <v>2.5649439626667628E-3</v>
+      </c>
+      <c r="BG63">
+        <f t="shared" si="24"/>
+        <v>2.2230760702519996E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>134</v>
       </c>
@@ -10004,6 +10929,9 @@
       </c>
       <c r="R64" t="s">
         <v>137</v>
+      </c>
+      <c r="AG64">
+        <v>50</v>
       </c>
       <c r="AH64">
         <v>2015</v>
@@ -10052,8 +10980,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW64">
+        <v>50</v>
+      </c>
+      <c r="AX64">
+        <v>2015</v>
+      </c>
+      <c r="AY64">
+        <v>0.11932297747701652</v>
+      </c>
+      <c r="AZ64">
+        <v>0.46260369865107809</v>
+      </c>
+      <c r="BA64">
+        <v>0.29620190409360969</v>
+      </c>
+      <c r="BB64">
+        <v>7.0559592420107342E-2</v>
+      </c>
+      <c r="BC64">
+        <v>2.9263027584974299E-2</v>
+      </c>
+      <c r="BD64">
+        <v>9.3093221611060973E-3</v>
+      </c>
+      <c r="BE64">
+        <v>6.5035577775107954E-3</v>
+      </c>
+      <c r="BF64">
+        <v>3.3499320115986334E-3</v>
+      </c>
+      <c r="BG64">
+        <f t="shared" si="24"/>
+        <v>2.8859878229984736E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>138</v>
       </c>
@@ -10107,6 +11069,9 @@
       </c>
       <c r="R65" t="s">
         <v>141</v>
+      </c>
+      <c r="AG65">
+        <v>50</v>
       </c>
       <c r="AH65">
         <v>2016</v>
@@ -10155,8 +11120,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW65">
+        <v>50</v>
+      </c>
+      <c r="AX65">
+        <v>2016</v>
+      </c>
+      <c r="AY65">
+        <v>0.12084631598848306</v>
+      </c>
+      <c r="AZ65">
+        <v>0.71007705498910367</v>
+      </c>
+      <c r="BA65">
+        <v>0.10024324010966026</v>
+      </c>
+      <c r="BB65">
+        <v>2.9577156659273733E-2</v>
+      </c>
+      <c r="BC65">
+        <v>1.780715489274793E-2</v>
+      </c>
+      <c r="BD65">
+        <v>1.1599478569257006E-2</v>
+      </c>
+      <c r="BE65">
+        <v>6.2341607992485127E-3</v>
+      </c>
+      <c r="BF65">
+        <v>2.6484913104160412E-3</v>
+      </c>
+      <c r="BG65">
+        <f t="shared" si="24"/>
+        <v>9.6694668180999995E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>142</v>
       </c>
@@ -10210,6 +11209,9 @@
       </c>
       <c r="R66" t="s">
         <v>145</v>
+      </c>
+      <c r="AG66">
+        <v>50</v>
       </c>
       <c r="AH66">
         <v>2017</v>
@@ -10258,8 +11260,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW66">
+        <v>50</v>
+      </c>
+      <c r="AX66">
+        <v>2017</v>
+      </c>
+      <c r="AY66">
+        <v>0.16144781831335123</v>
+      </c>
+      <c r="AZ66">
+        <v>0.35183350107339112</v>
+      </c>
+      <c r="BA66">
+        <v>0.2728285411102927</v>
+      </c>
+      <c r="BB66">
+        <v>0.12977636738152581</v>
+      </c>
+      <c r="BC66">
+        <v>4.7946293732230083E-2</v>
+      </c>
+      <c r="BD66">
+        <v>2.1357940908225868E-2</v>
+      </c>
+      <c r="BE66">
+        <v>9.4517398986345806E-3</v>
+      </c>
+      <c r="BF66">
+        <v>3.3214341699114368E-3</v>
+      </c>
+      <c r="BG66">
+        <f t="shared" si="24"/>
+        <v>2.0363634124372677E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>146</v>
       </c>
@@ -10313,6 +11349,9 @@
       </c>
       <c r="R67" t="s">
         <v>149</v>
+      </c>
+      <c r="AG67">
+        <v>50</v>
       </c>
       <c r="AH67">
         <v>2018</v>
@@ -10361,8 +11400,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW67">
+        <v>50</v>
+      </c>
+      <c r="AX67">
+        <v>2018</v>
+      </c>
+      <c r="AY67">
+        <v>3.6597912150439206E-2</v>
+      </c>
+      <c r="AZ67">
+        <v>0.29353680946863187</v>
+      </c>
+      <c r="BA67">
+        <v>0.45215862491748393</v>
+      </c>
+      <c r="BB67">
+        <v>0.16336520024479009</v>
+      </c>
+      <c r="BC67">
+        <v>3.2222495008467335E-2</v>
+      </c>
+      <c r="BD67">
+        <v>1.6391380976019998E-2</v>
+      </c>
+      <c r="BE67">
+        <v>3.8522104887512509E-3</v>
+      </c>
+      <c r="BF67">
+        <v>8.4122309758383933E-4</v>
+      </c>
+      <c r="BG67">
+        <f t="shared" si="24"/>
+        <v>1.0341436478325076E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>150</v>
       </c>
@@ -10416,6 +11489,9 @@
       </c>
       <c r="R68" t="s">
         <v>153</v>
+      </c>
+      <c r="AG68">
+        <v>50</v>
       </c>
       <c r="AH68">
         <v>2019</v>
@@ -10464,8 +11540,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW68">
+        <v>50</v>
+      </c>
+      <c r="AX68">
+        <v>2019</v>
+      </c>
+      <c r="AY68">
+        <v>9.5062736694461317E-2</v>
+      </c>
+      <c r="AZ68">
+        <v>0.48329154969330695</v>
+      </c>
+      <c r="BA68">
+        <v>0.27245515025848294</v>
+      </c>
+      <c r="BB68">
+        <v>8.7950189135307069E-2</v>
+      </c>
+      <c r="BC68">
+        <v>3.2772435835363024E-2</v>
+      </c>
+      <c r="BD68">
+        <v>1.6129123935043246E-2</v>
+      </c>
+      <c r="BE68">
+        <v>7.4590873733919611E-3</v>
+      </c>
+      <c r="BF68">
+        <v>2.8706168292571472E-3</v>
+      </c>
+      <c r="BG68">
+        <f t="shared" si="24"/>
+        <v>2.0091102453862922E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -10519,6 +11629,9 @@
       </c>
       <c r="R69" t="s">
         <v>157</v>
+      </c>
+      <c r="AG69">
+        <v>50</v>
       </c>
       <c r="AH69">
         <v>2020</v>
@@ -10567,8 +11680,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW69">
+        <v>50</v>
+      </c>
+      <c r="AX69">
+        <v>2020</v>
+      </c>
+      <c r="AY69">
+        <v>0.45100804829484947</v>
+      </c>
+      <c r="AZ69">
+        <v>0.34507851295770231</v>
+      </c>
+      <c r="BA69">
+        <v>0.14158573749201975</v>
+      </c>
+      <c r="BB69">
+        <v>4.2143266911392661E-2</v>
+      </c>
+      <c r="BC69">
+        <v>1.404303759671539E-2</v>
+      </c>
+      <c r="BD69">
+        <v>5.2891934900463466E-3</v>
+      </c>
+      <c r="BE69">
+        <v>6.4565753750675959E-4</v>
+      </c>
+      <c r="BF69">
+        <v>1.9034059486467059E-4</v>
+      </c>
+      <c r="BG69">
+        <f t="shared" si="24"/>
+        <v>1.6205124902315878E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>158</v>
       </c>
@@ -10622,6 +11769,9 @@
       </c>
       <c r="R70" t="s">
         <v>161</v>
+      </c>
+      <c r="AG70">
+        <v>50</v>
       </c>
       <c r="AH70">
         <v>2021</v>
@@ -10670,8 +11820,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW70">
+        <v>50</v>
+      </c>
+      <c r="AX70">
+        <v>2021</v>
+      </c>
+      <c r="AY70">
+        <v>0.48245356414846435</v>
+      </c>
+      <c r="AZ70">
+        <v>0.23632728617567836</v>
+      </c>
+      <c r="BA70">
+        <v>0.21466560674826718</v>
+      </c>
+      <c r="BB70">
+        <v>3.5808625868391446E-2</v>
+      </c>
+      <c r="BC70">
+        <v>2.1811711334515007E-2</v>
+      </c>
+      <c r="BD70">
+        <v>6.9082208492182223E-3</v>
+      </c>
+      <c r="BE70">
+        <v>1.734958217677037E-3</v>
+      </c>
+      <c r="BF70">
+        <v>2.3524289593714479E-4</v>
+      </c>
+      <c r="BG70">
+        <f t="shared" si="24"/>
+        <v>5.4783761851269178E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>162</v>
       </c>
@@ -10725,6 +11909,9 @@
       </c>
       <c r="R71" t="s">
         <v>165</v>
+      </c>
+      <c r="AG71">
+        <v>50</v>
       </c>
       <c r="AH71">
         <v>2022</v>
@@ -10773,8 +11960,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW71">
+        <v>50</v>
+      </c>
+      <c r="AX71">
+        <v>2022</v>
+      </c>
+      <c r="AY71">
+        <v>0.13452486227576471</v>
+      </c>
+      <c r="AZ71">
+        <v>0.45787412395306804</v>
+      </c>
+      <c r="BA71">
+        <v>0.29387968570107187</v>
+      </c>
+      <c r="BB71">
+        <v>6.4210330730117504E-2</v>
+      </c>
+      <c r="BC71">
+        <v>3.667885063155258E-2</v>
+      </c>
+      <c r="BD71">
+        <v>8.758936747386219E-3</v>
+      </c>
+      <c r="BE71">
+        <v>3.532077756084728E-3</v>
+      </c>
+      <c r="BF71">
+        <v>4.4147082156269452E-4</v>
+      </c>
+      <c r="BG71">
+        <f t="shared" si="24"/>
+        <v>9.9661383391664384E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>166</v>
       </c>
@@ -10828,6 +12049,9 @@
       </c>
       <c r="R72" t="s">
         <v>169</v>
+      </c>
+      <c r="AG72">
+        <v>50</v>
       </c>
       <c r="AH72">
         <v>2023</v>
@@ -10876,8 +12100,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW72">
+        <v>50</v>
+      </c>
+      <c r="AX72">
+        <v>2023</v>
+      </c>
+      <c r="AY72">
+        <v>0.21299702021393582</v>
+      </c>
+      <c r="AZ72">
+        <v>4.4599583484097108E-2</v>
+      </c>
+      <c r="BA72">
+        <v>0.43357960552339431</v>
+      </c>
+      <c r="BB72">
+        <v>0.22430807849480486</v>
+      </c>
+      <c r="BC72">
+        <v>5.9164549688638129E-2</v>
+      </c>
+      <c r="BD72">
+        <v>1.9009520110410509E-2</v>
+      </c>
+      <c r="BE72">
+        <v>4.8473465592770533E-3</v>
+      </c>
+      <c r="BF72">
+        <v>7.4003386509957419E-4</v>
+      </c>
+      <c r="BG72">
+        <f t="shared" si="24"/>
+        <v>7.542620603426984E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>170</v>
       </c>
@@ -10931,6 +12189,9 @@
       </c>
       <c r="R73" t="s">
         <v>173</v>
+      </c>
+      <c r="AG73">
+        <v>50</v>
       </c>
       <c r="AH73">
         <v>2024</v>
@@ -10979,8 +12240,42 @@
         <f t="shared" si="23"/>
         <v>New</v>
       </c>
-    </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AW73">
+        <v>50</v>
+      </c>
+      <c r="AX73">
+        <v>2024</v>
+      </c>
+      <c r="AY73">
+        <v>0.10492490207626529</v>
+      </c>
+      <c r="AZ73">
+        <v>0.25330857419357916</v>
+      </c>
+      <c r="BA73">
+        <v>0.40990405406435299</v>
+      </c>
+      <c r="BB73">
+        <v>0.17227158073273602</v>
+      </c>
+      <c r="BC73">
+        <v>4.5696431987400567E-2</v>
+      </c>
+      <c r="BD73">
+        <v>1.1512703641771906E-2</v>
+      </c>
+      <c r="BE73">
+        <v>2.1532168246178617E-3</v>
+      </c>
+      <c r="BF73">
+        <v>1.7250796882499418E-4</v>
+      </c>
+      <c r="BG73">
+        <f t="shared" si="24"/>
+        <v>5.6028510451104616E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>174</v>
       </c>
@@ -11036,12 +12331,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:59" x14ac:dyDescent="0.2">
       <c r="E75" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>179</v>
       </c>
@@ -11097,7 +12392,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>183</v>
       </c>
@@ -11153,7 +12448,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -11209,7 +12504,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>191</v>
       </c>
@@ -11265,7 +12560,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>195</v>
       </c>
@@ -16498,6 +17793,16 @@
   </sheetData>
   <conditionalFormatting sqref="U4:AD38">
     <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI4:AQ38 AS4:AS38">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -16516,16 +17821,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI4:AQ38 AS4:AS38">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -16533,10 +17828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38AC0BA-9238-4988-A35D-0926280AB7AA}">
-  <dimension ref="A1:AJ143"/>
+  <dimension ref="A1:AW143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView topLeftCell="S3" workbookViewId="0">
+      <selection activeCell="AW31" sqref="AM31:AW57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17683,7 +18978,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>21</v>
       </c>
@@ -17763,7 +19058,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>22</v>
       </c>
@@ -17843,7 +19138,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>23</v>
       </c>
@@ -17923,7 +19218,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>24</v>
       </c>
@@ -18003,7 +19298,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>25</v>
       </c>
@@ -18083,7 +19378,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>26</v>
       </c>
@@ -18163,7 +19458,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>27</v>
       </c>
@@ -18243,7 +19538,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>28</v>
       </c>
@@ -18323,7 +19618,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>29</v>
       </c>
@@ -18403,7 +19698,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>30</v>
       </c>
@@ -18483,7 +19778,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>31</v>
       </c>
@@ -18563,7 +19858,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>32</v>
       </c>
@@ -18643,7 +19938,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>33</v>
       </c>
@@ -18723,7 +20018,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>34</v>
       </c>
@@ -18803,7 +20098,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
         <v>36</v>
       </c>
@@ -18847,8 +20142,42 @@
       <c r="AJ31" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM31">
+        <v>50</v>
+      </c>
+      <c r="AN31">
+        <v>1997</v>
+      </c>
+      <c r="AO31">
+        <v>2.4010166443328438E-4</v>
+      </c>
+      <c r="AP31">
+        <v>5.7452996197930664E-3</v>
+      </c>
+      <c r="AQ31">
+        <v>6.6370879812007386E-2</v>
+      </c>
+      <c r="AR31">
+        <v>0.24076996044506743</v>
+      </c>
+      <c r="AS31">
+        <v>0.34954784804866862</v>
+      </c>
+      <c r="AT31">
+        <v>0.20179712160595761</v>
+      </c>
+      <c r="AU31">
+        <v>8.0642092534665158E-2</v>
+      </c>
+      <c r="AV31">
+        <v>3.2524653276863415E-2</v>
+      </c>
+      <c r="AW31">
+        <f>SUM(AH31:AI31)</f>
+        <v>2.2362042992544094E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>312</v>
       </c>
@@ -18943,8 +20272,42 @@
       <c r="AJ32" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM32">
+        <v>50</v>
+      </c>
+      <c r="AN32">
+        <v>1998</v>
+      </c>
+      <c r="AO32">
+        <v>2.3729756833739315E-4</v>
+      </c>
+      <c r="AP32">
+        <v>8.4657039207790517E-3</v>
+      </c>
+      <c r="AQ32">
+        <v>4.3063970812600341E-2</v>
+      </c>
+      <c r="AR32">
+        <v>0.15359044659002039</v>
+      </c>
+      <c r="AS32">
+        <v>0.36307028296512311</v>
+      </c>
+      <c r="AT32">
+        <v>0.25387917335678345</v>
+      </c>
+      <c r="AU32">
+        <v>0.10344536613751121</v>
+      </c>
+      <c r="AV32">
+        <v>4.1071022262593293E-2</v>
+      </c>
+      <c r="AW32">
+        <f t="shared" ref="AW32:AW57" si="1">SUM(AH32:AI32)</f>
+        <v>3.317673638625189E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>314</v>
       </c>
@@ -19039,8 +20402,42 @@
       <c r="AJ33" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM33">
+        <v>50</v>
+      </c>
+      <c r="AN33">
+        <v>1999</v>
+      </c>
+      <c r="AO33">
+        <v>2.165728496528279E-3</v>
+      </c>
+      <c r="AP33">
+        <v>1.7387503239774508E-2</v>
+      </c>
+      <c r="AQ33">
+        <v>0.12843496461298592</v>
+      </c>
+      <c r="AR33">
+        <v>0.20718117504776457</v>
+      </c>
+      <c r="AS33">
+        <v>0.26942788300319287</v>
+      </c>
+      <c r="AT33">
+        <v>0.18923653011298613</v>
+      </c>
+      <c r="AU33">
+        <v>0.10069497138883141</v>
+      </c>
+      <c r="AV33">
+        <v>5.6435360323579452E-2</v>
+      </c>
+      <c r="AW33">
+        <f t="shared" si="1"/>
+        <v>2.9035883774356765E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>316</v>
       </c>
@@ -19135,8 +20532,42 @@
       <c r="AJ34" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM34">
+        <v>50</v>
+      </c>
+      <c r="AN34">
+        <v>2000</v>
+      </c>
+      <c r="AO34">
+        <v>2.7342229162682945E-4</v>
+      </c>
+      <c r="AP34">
+        <v>5.268101491630932E-3</v>
+      </c>
+      <c r="AQ34">
+        <v>3.8288392063364735E-2</v>
+      </c>
+      <c r="AR34">
+        <v>0.18730262635714295</v>
+      </c>
+      <c r="AS34">
+        <v>0.33577426280754413</v>
+      </c>
+      <c r="AT34">
+        <v>0.30738678765241162</v>
+      </c>
+      <c r="AU34">
+        <v>7.6770077468869116E-2</v>
+      </c>
+      <c r="AV34">
+        <v>4.079369339198665E-2</v>
+      </c>
+      <c r="AW34">
+        <f t="shared" si="1"/>
+        <v>8.1426364754231054E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>318</v>
       </c>
@@ -19231,8 +20662,42 @@
       <c r="AJ35" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM35">
+        <v>50</v>
+      </c>
+      <c r="AN35">
+        <v>2001</v>
+      </c>
+      <c r="AO35">
+        <v>1.5176733729391572E-3</v>
+      </c>
+      <c r="AP35">
+        <v>2.6774666114771552E-2</v>
+      </c>
+      <c r="AQ35">
+        <v>0.12529144837228917</v>
+      </c>
+      <c r="AR35">
+        <v>0.24983825575584648</v>
+      </c>
+      <c r="AS35">
+        <v>0.3159954889898634</v>
+      </c>
+      <c r="AT35">
+        <v>0.18986523990206139</v>
+      </c>
+      <c r="AU35">
+        <v>5.297253167648204E-2</v>
+      </c>
+      <c r="AV35">
+        <v>2.5922142073374285E-2</v>
+      </c>
+      <c r="AW35">
+        <f t="shared" si="1"/>
+        <v>1.1822553742372646E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>320</v>
       </c>
@@ -19327,8 +20792,42 @@
       <c r="AJ36" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM36">
+        <v>50</v>
+      </c>
+      <c r="AN36">
+        <v>2002</v>
+      </c>
+      <c r="AO36">
+        <v>3.5035370858669011E-4</v>
+      </c>
+      <c r="AP36">
+        <v>6.3854219869462867E-2</v>
+      </c>
+      <c r="AQ36">
+        <v>0.24034506707009723</v>
+      </c>
+      <c r="AR36">
+        <v>0.18824565549620745</v>
+      </c>
+      <c r="AS36">
+        <v>0.3013149575908437</v>
+      </c>
+      <c r="AT36">
+        <v>0.13662447711988612</v>
+      </c>
+      <c r="AU36">
+        <v>4.1428581059752591E-2</v>
+      </c>
+      <c r="AV36">
+        <v>1.7371232700017003E-2</v>
+      </c>
+      <c r="AW36">
+        <f t="shared" si="1"/>
+        <v>1.046545538514629E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>322</v>
       </c>
@@ -19423,8 +20922,42 @@
       <c r="AJ37" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM37">
+        <v>50</v>
+      </c>
+      <c r="AN37">
+        <v>2003</v>
+      </c>
+      <c r="AO37">
+        <v>3.8489621736747517E-3</v>
+      </c>
+      <c r="AP37">
+        <v>3.5476610272618107E-2</v>
+      </c>
+      <c r="AQ37">
+        <v>0.22418699126268363</v>
+      </c>
+      <c r="AR37">
+        <v>0.25922006858705349</v>
+      </c>
+      <c r="AS37">
+        <v>0.25707509737133971</v>
+      </c>
+      <c r="AT37">
+        <v>0.1435643838104953</v>
+      </c>
+      <c r="AU37">
+        <v>4.2853588641117595E-2</v>
+      </c>
+      <c r="AV37">
+        <v>1.5504444802028948E-2</v>
+      </c>
+      <c r="AW37">
+        <f t="shared" si="1"/>
+        <v>1.8269853078988395E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>324</v>
       </c>
@@ -19519,8 +21052,42 @@
       <c r="AJ38" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM38">
+        <v>50</v>
+      </c>
+      <c r="AN38">
+        <v>2004</v>
+      </c>
+      <c r="AO38">
+        <v>2.4282242123477906E-4</v>
+      </c>
+      <c r="AP38">
+        <v>1.8746782300958411E-2</v>
+      </c>
+      <c r="AQ38">
+        <v>9.419196639598619E-2</v>
+      </c>
+      <c r="AR38">
+        <v>0.36647494441904299</v>
+      </c>
+      <c r="AS38">
+        <v>0.31236848918286336</v>
+      </c>
+      <c r="AT38">
+        <v>0.1375878248057773</v>
+      </c>
+      <c r="AU38">
+        <v>4.9377948751160985E-2</v>
+      </c>
+      <c r="AV38">
+        <v>1.4058056675707795E-2</v>
+      </c>
+      <c r="AW38">
+        <f t="shared" si="1"/>
+        <v>6.9511650472681517E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>326</v>
       </c>
@@ -19615,8 +21182,42 @@
       <c r="AJ39" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM39">
+        <v>50</v>
+      </c>
+      <c r="AN39">
+        <v>2005</v>
+      </c>
+      <c r="AO39">
+        <v>1.2754374229215233E-5</v>
+      </c>
+      <c r="AP39">
+        <v>1.5157285006130526E-3</v>
+      </c>
+      <c r="AQ39">
+        <v>5.1287220029897281E-2</v>
+      </c>
+      <c r="AR39">
+        <v>0.38741470023106295</v>
+      </c>
+      <c r="AS39">
+        <v>0.4028863678346129</v>
+      </c>
+      <c r="AT39">
+        <v>0.12221361052591929</v>
+      </c>
+      <c r="AU39">
+        <v>2.5515030321864647E-2</v>
+      </c>
+      <c r="AV39">
+        <v>3.1887634110914533E-3</v>
+      </c>
+      <c r="AW39">
+        <f t="shared" si="1"/>
+        <v>5.9658247707092601E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -19711,8 +21312,42 @@
       <c r="AJ40" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM40">
+        <v>50</v>
+      </c>
+      <c r="AN40">
+        <v>2006</v>
+      </c>
+      <c r="AO40">
+        <v>1.73070317489635E-5</v>
+      </c>
+      <c r="AP40">
+        <v>2.7024126778160697E-3</v>
+      </c>
+      <c r="AQ40">
+        <v>6.3364255966825586E-2</v>
+      </c>
+      <c r="AR40">
+        <v>0.33198120486595195</v>
+      </c>
+      <c r="AS40">
+        <v>0.43312795928259601</v>
+      </c>
+      <c r="AT40">
+        <v>0.12920920389984519</v>
+      </c>
+      <c r="AU40">
+        <v>3.3419211917327621E-2</v>
+      </c>
+      <c r="AV40">
+        <v>4.5961175385324845E-3</v>
+      </c>
+      <c r="AW40">
+        <f t="shared" si="1"/>
+        <v>1.5823268193559826E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>330</v>
       </c>
@@ -19807,8 +21442,42 @@
       <c r="AJ41" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM41">
+        <v>50</v>
+      </c>
+      <c r="AN41">
+        <v>2007</v>
+      </c>
+      <c r="AO41">
+        <v>2.768168533988274E-4</v>
+      </c>
+      <c r="AP41">
+        <v>1.0304855406105028E-2</v>
+      </c>
+      <c r="AQ41">
+        <v>0.10373741890098241</v>
+      </c>
+      <c r="AR41">
+        <v>0.29416709980125033</v>
+      </c>
+      <c r="AS41">
+        <v>0.30719978258195813</v>
+      </c>
+      <c r="AT41">
+        <v>0.15994423669981372</v>
+      </c>
+      <c r="AU41">
+        <v>7.663065930567714E-2</v>
+      </c>
+      <c r="AV41">
+        <v>3.6596781092834652E-2</v>
+      </c>
+      <c r="AW41">
+        <f t="shared" si="1"/>
+        <v>1.1142349357979866E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>332</v>
       </c>
@@ -19903,8 +21572,42 @@
       <c r="AJ42" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM42">
+        <v>50</v>
+      </c>
+      <c r="AN42">
+        <v>2008</v>
+      </c>
+      <c r="AO42">
+        <v>1.1888180327866071E-4</v>
+      </c>
+      <c r="AP42">
+        <v>1.3397185965485902E-2</v>
+      </c>
+      <c r="AQ42">
+        <v>9.3534279768985235E-2</v>
+      </c>
+      <c r="AR42">
+        <v>0.24208346923134122</v>
+      </c>
+      <c r="AS42">
+        <v>0.36628904764633891</v>
+      </c>
+      <c r="AT42">
+        <v>0.19491080038844366</v>
+      </c>
+      <c r="AU42">
+        <v>5.8894814082862595E-2</v>
+      </c>
+      <c r="AV42">
+        <v>1.709827551065787E-2</v>
+      </c>
+      <c r="AW42">
+        <f t="shared" si="1"/>
+        <v>1.3673245602606153E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>334</v>
       </c>
@@ -19999,8 +21702,42 @@
       <c r="AJ43" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM43">
+        <v>50</v>
+      </c>
+      <c r="AN43">
+        <v>2009</v>
+      </c>
+      <c r="AO43">
+        <v>2.2267369350145217E-4</v>
+      </c>
+      <c r="AP43">
+        <v>2.3002867783960143E-2</v>
+      </c>
+      <c r="AQ43">
+        <v>0.14199290567677009</v>
+      </c>
+      <c r="AR43">
+        <v>0.26840806115995064</v>
+      </c>
+      <c r="AS43">
+        <v>0.29338796807842804</v>
+      </c>
+      <c r="AT43">
+        <v>0.15165483215516651</v>
+      </c>
+      <c r="AU43">
+        <v>6.8218158494356154E-2</v>
+      </c>
+      <c r="AV43">
+        <v>2.7178306061751145E-2</v>
+      </c>
+      <c r="AW43">
+        <f t="shared" si="1"/>
+        <v>2.593422689611577E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>336</v>
       </c>
@@ -20095,8 +21832,42 @@
       <c r="AJ44" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM44">
+        <v>50</v>
+      </c>
+      <c r="AN44">
+        <v>2010</v>
+      </c>
+      <c r="AO44">
+        <v>8.713776633174489E-5</v>
+      </c>
+      <c r="AP44">
+        <v>1.418262875703169E-2</v>
+      </c>
+      <c r="AQ44">
+        <v>0.13915661856645306</v>
+      </c>
+      <c r="AR44">
+        <v>0.43906733517014146</v>
+      </c>
+      <c r="AS44">
+        <v>0.27902405981932071</v>
+      </c>
+      <c r="AT44">
+        <v>9.2198486942985755E-2</v>
+      </c>
+      <c r="AU44">
+        <v>2.196192292742772E-2</v>
+      </c>
+      <c r="AV44">
+        <v>9.0277236940882865E-3</v>
+      </c>
+      <c r="AW44">
+        <f t="shared" si="1"/>
+        <v>5.2940863562195191E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>338</v>
       </c>
@@ -20191,8 +21962,42 @@
       <c r="AJ45" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM45">
+        <v>50</v>
+      </c>
+      <c r="AN45">
+        <v>2011</v>
+      </c>
+      <c r="AO45">
+        <v>2.082563538085107E-5</v>
+      </c>
+      <c r="AP45">
+        <v>4.3268419669947912E-3</v>
+      </c>
+      <c r="AQ45">
+        <v>4.8926543787083873E-2</v>
+      </c>
+      <c r="AR45">
+        <v>0.22283380000256711</v>
+      </c>
+      <c r="AS45">
+        <v>0.27819965763063992</v>
+      </c>
+      <c r="AT45">
+        <v>0.18985596179670469</v>
+      </c>
+      <c r="AU45">
+        <v>0.13503581346727109</v>
+      </c>
+      <c r="AV45">
+        <v>5.5832731628645625E-2</v>
+      </c>
+      <c r="AW45">
+        <f t="shared" si="1"/>
+        <v>6.4967824084712092E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>340</v>
       </c>
@@ -20287,8 +22092,42 @@
       <c r="AJ46" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM46">
+        <v>50</v>
+      </c>
+      <c r="AN46">
+        <v>2012</v>
+      </c>
+      <c r="AO46">
+        <v>3.2201196310819701E-4</v>
+      </c>
+      <c r="AP46">
+        <v>3.1453047454347023E-2</v>
+      </c>
+      <c r="AQ46">
+        <v>0.24531242366920453</v>
+      </c>
+      <c r="AR46">
+        <v>0.16796178061408884</v>
+      </c>
+      <c r="AS46">
+        <v>0.34311300630063912</v>
+      </c>
+      <c r="AT46">
+        <v>0.11514402042837131</v>
+      </c>
+      <c r="AU46">
+        <v>4.8928311949270345E-2</v>
+      </c>
+      <c r="AV46">
+        <v>1.9866565696523703E-2</v>
+      </c>
+      <c r="AW46">
+        <f t="shared" si="1"/>
+        <v>2.7898831924446921E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>342</v>
       </c>
@@ -20383,8 +22222,42 @@
       <c r="AJ47" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM47">
+        <v>50</v>
+      </c>
+      <c r="AN47">
+        <v>2013</v>
+      </c>
+      <c r="AO47">
+        <v>1.2538664899458695E-4</v>
+      </c>
+      <c r="AP47">
+        <v>1.317577793983773E-2</v>
+      </c>
+      <c r="AQ47">
+        <v>0.16668395315103407</v>
+      </c>
+      <c r="AR47">
+        <v>0.25739845097187181</v>
+      </c>
+      <c r="AS47">
+        <v>0.29745467893911864</v>
+      </c>
+      <c r="AT47">
+        <v>0.1378547722429318</v>
+      </c>
+      <c r="AU47">
+        <v>6.9195430044729625E-2</v>
+      </c>
+      <c r="AV47">
+        <v>2.5558994172871611E-2</v>
+      </c>
+      <c r="AW47">
+        <f t="shared" si="1"/>
+        <v>3.2552555888610071E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>344</v>
       </c>
@@ -20479,8 +22352,42 @@
       <c r="AJ48" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM48">
+        <v>50</v>
+      </c>
+      <c r="AN48">
+        <v>2014</v>
+      </c>
+      <c r="AO48">
+        <v>1.6438523076786461E-4</v>
+      </c>
+      <c r="AP48">
+        <v>3.8681052864505919E-2</v>
+      </c>
+      <c r="AQ48">
+        <v>0.1657743708759977</v>
+      </c>
+      <c r="AR48">
+        <v>0.23652630111143713</v>
+      </c>
+      <c r="AS48">
+        <v>0.20683139862814001</v>
+      </c>
+      <c r="AT48">
+        <v>0.17403441364061306</v>
+      </c>
+      <c r="AU48">
+        <v>0.13870588990241789</v>
+      </c>
+      <c r="AV48">
+        <v>2.4074214044131806E-2</v>
+      </c>
+      <c r="AW48">
+        <f t="shared" si="1"/>
+        <v>1.5207973701988831E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>346</v>
       </c>
@@ -20575,8 +22482,42 @@
       <c r="AJ49" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM49">
+        <v>50</v>
+      </c>
+      <c r="AN49">
+        <v>2015</v>
+      </c>
+      <c r="AO49">
+        <v>2.0491945072818573E-4</v>
+      </c>
+      <c r="AP49">
+        <v>1.5267885385035783E-2</v>
+      </c>
+      <c r="AQ49">
+        <v>0.21826536847563818</v>
+      </c>
+      <c r="AR49">
+        <v>0.31177404373510009</v>
+      </c>
+      <c r="AS49">
+        <v>0.26298456022891759</v>
+      </c>
+      <c r="AT49">
+        <v>8.8605942912099556E-2</v>
+      </c>
+      <c r="AU49">
+        <v>6.067754027606307E-2</v>
+      </c>
+      <c r="AV49">
+        <v>2.3973173143162278E-2</v>
+      </c>
+      <c r="AW49">
+        <f t="shared" si="1"/>
+        <v>1.8246566393255125E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>348</v>
       </c>
@@ -20671,8 +22612,42 @@
       <c r="AJ50" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM50">
+        <v>50</v>
+      </c>
+      <c r="AN50">
+        <v>2016</v>
+      </c>
+      <c r="AO50">
+        <v>1.262550549748396E-3</v>
+      </c>
+      <c r="AP50">
+        <v>0.12449627518123645</v>
+      </c>
+      <c r="AQ50">
+        <v>0.30386109813890916</v>
+      </c>
+      <c r="AR50">
+        <v>0.27141487617271065</v>
+      </c>
+      <c r="AS50">
+        <v>0.14776801896358518</v>
+      </c>
+      <c r="AT50">
+        <v>9.2625091645196944E-2</v>
+      </c>
+      <c r="AU50">
+        <v>3.6968964804118876E-2</v>
+      </c>
+      <c r="AV50">
+        <v>1.5349905599502148E-2</v>
+      </c>
+      <c r="AW50">
+        <f t="shared" si="1"/>
+        <v>6.2532189449922594E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>350</v>
       </c>
@@ -20767,8 +22742,42 @@
       <c r="AJ51" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM51">
+        <v>50</v>
+      </c>
+      <c r="AN51">
+        <v>2017</v>
+      </c>
+      <c r="AO51">
+        <v>4.4244954767795375E-4</v>
+      </c>
+      <c r="AP51">
+        <v>7.366659331949825E-2</v>
+      </c>
+      <c r="AQ51">
+        <v>0.35049564488461049</v>
+      </c>
+      <c r="AR51">
+        <v>0.3086380105870441</v>
+      </c>
+      <c r="AS51">
+        <v>0.16790944236577909</v>
+      </c>
+      <c r="AT51">
+        <v>6.739260825756363E-2</v>
+      </c>
+      <c r="AU51">
+        <v>2.2771937106893587E-2</v>
+      </c>
+      <c r="AV51">
+        <v>5.5918961268106564E-3</v>
+      </c>
+      <c r="AW51">
+        <f t="shared" si="1"/>
+        <v>3.0914178041223923E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>352</v>
       </c>
@@ -20863,8 +22872,42 @@
       <c r="AJ52" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM52">
+        <v>50</v>
+      </c>
+      <c r="AN52">
+        <v>2018</v>
+      </c>
+      <c r="AO52">
+        <v>1.5840489272444562E-4</v>
+      </c>
+      <c r="AP52">
+        <v>0.10216296273610262</v>
+      </c>
+      <c r="AQ52">
+        <v>0.17536675664773613</v>
+      </c>
+      <c r="AR52">
+        <v>0.45109301801325913</v>
+      </c>
+      <c r="AS52">
+        <v>0.18847091257066878</v>
+      </c>
+      <c r="AT52">
+        <v>6.1279783490561977E-2</v>
+      </c>
+      <c r="AU52">
+        <v>1.3316397313379212E-2</v>
+      </c>
+      <c r="AV52">
+        <v>3.7666229388575601E-3</v>
+      </c>
+      <c r="AW52">
+        <f t="shared" si="1"/>
+        <v>4.3851413967100489E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>354</v>
       </c>
@@ -20959,8 +23002,42 @@
       <c r="AJ53" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM53">
+        <v>50</v>
+      </c>
+      <c r="AN53">
+        <v>2019</v>
+      </c>
+      <c r="AO53">
+        <v>9.5129487674710351E-5</v>
+      </c>
+      <c r="AP53">
+        <v>5.9519360662821937E-2</v>
+      </c>
+      <c r="AQ53">
+        <v>0.30030718879893104</v>
+      </c>
+      <c r="AR53">
+        <v>0.34220705615639568</v>
+      </c>
+      <c r="AS53">
+        <v>0.18151042216905808</v>
+      </c>
+      <c r="AT53">
+        <v>7.1137630966332188E-2</v>
+      </c>
+      <c r="AU53">
+        <v>2.9923508413682156E-2</v>
+      </c>
+      <c r="AV53">
+        <v>9.1996643060286657E-3</v>
+      </c>
+      <c r="AW53">
+        <f t="shared" si="1"/>
+        <v>6.1000390390756505E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>356</v>
       </c>
@@ -21055,8 +23132,42 @@
       <c r="AJ54" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM54">
+        <v>50</v>
+      </c>
+      <c r="AN54">
+        <v>2020</v>
+      </c>
+      <c r="AO54">
+        <v>2.1236575914878853E-3</v>
+      </c>
+      <c r="AP54">
+        <v>0.10903214840668243</v>
+      </c>
+      <c r="AQ54">
+        <v>0.39982520588312359</v>
+      </c>
+      <c r="AR54">
+        <v>0.32191017596641608</v>
+      </c>
+      <c r="AS54">
+        <v>0.1306313367391882</v>
+      </c>
+      <c r="AT54">
+        <v>3.0484517695859924E-2</v>
+      </c>
+      <c r="AU54">
+        <v>4.0279547861779121E-3</v>
+      </c>
+      <c r="AV54">
+        <v>1.7796428850280546E-3</v>
+      </c>
+      <c r="AW54">
+        <f t="shared" si="1"/>
+        <v>1.85360046035817E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>358</v>
       </c>
@@ -21151,8 +23262,42 @@
       <c r="AJ55" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM55">
+        <v>50</v>
+      </c>
+      <c r="AN55">
+        <v>2021</v>
+      </c>
+      <c r="AO55">
+        <v>5.9478336655172017E-3</v>
+      </c>
+      <c r="AP55">
+        <v>9.5342403019649108E-2</v>
+      </c>
+      <c r="AQ55">
+        <v>0.34985476967532442</v>
+      </c>
+      <c r="AR55">
+        <v>0.29622060621266477</v>
+      </c>
+      <c r="AS55">
+        <v>0.20263423579289774</v>
+      </c>
+      <c r="AT55">
+        <v>3.7964066830462904E-2</v>
+      </c>
+      <c r="AU55">
+        <v>9.1916199509124562E-3</v>
+      </c>
+      <c r="AV55">
+        <v>1.9194085297804804E-3</v>
+      </c>
+      <c r="AW55">
+        <f t="shared" si="1"/>
+        <v>9.2505632279068562E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>360</v>
       </c>
@@ -21247,8 +23392,42 @@
       <c r="AJ56" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM56">
+        <v>50</v>
+      </c>
+      <c r="AN56">
+        <v>2022</v>
+      </c>
+      <c r="AO56">
+        <v>4.4612655637283052E-3</v>
+      </c>
+      <c r="AP56">
+        <v>0.11144564992396902</v>
+      </c>
+      <c r="AQ56">
+        <v>0.39101121334908079</v>
+      </c>
+      <c r="AR56">
+        <v>0.29207833491866442</v>
+      </c>
+      <c r="AS56">
+        <v>0.15891719491506873</v>
+      </c>
+      <c r="AT56">
+        <v>3.0846685082937739E-2</v>
+      </c>
+      <c r="AU56">
+        <v>8.8557425797385642E-3</v>
+      </c>
+      <c r="AV56">
+        <v>1.6835308628370615E-3</v>
+      </c>
+      <c r="AW56">
+        <f t="shared" si="1"/>
+        <v>7.0038280397517565E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>362</v>
       </c>
@@ -21343,8 +23522,42 @@
       <c r="AJ57" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM57">
+        <v>50</v>
+      </c>
+      <c r="AN57">
+        <v>2023</v>
+      </c>
+      <c r="AO57">
+        <v>3.3444822939586415E-3</v>
+      </c>
+      <c r="AP57">
+        <v>7.141240400458309E-3</v>
+      </c>
+      <c r="AQ57">
+        <v>0.23591171874406625</v>
+      </c>
+      <c r="AR57">
+        <v>0.43082943523626016</v>
+      </c>
+      <c r="AS57">
+        <v>0.26569748305489904</v>
+      </c>
+      <c r="AT57">
+        <v>4.965254078165781E-2</v>
+      </c>
+      <c r="AU57">
+        <v>6.2231809887981285E-3</v>
+      </c>
+      <c r="AV57">
+        <v>5.3165127827847281E-4</v>
+      </c>
+      <c r="AW57">
+        <f t="shared" si="1"/>
+        <v>6.6826722162318351E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>364</v>
       </c>
@@ -21400,12 +23613,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:49" x14ac:dyDescent="0.2">
       <c r="E59" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>366</v>
       </c>
@@ -21461,7 +23674,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>368</v>
       </c>
@@ -21517,7 +23730,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -21573,7 +23786,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>372</v>
       </c>
@@ -21629,7 +23842,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>374</v>
       </c>

</xml_diff>